<commit_message>
Case 1, Case 2 setup and ready to run
</commit_message>
<xml_diff>
--- a/ClimateStudies/docsandreports/uRXClimateStudiesMasterFile.xlsx
+++ b/ClimateStudies/docsandreports/uRXClimateStudiesMasterFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f76ff82bf46bf64a/repo/homer/ClimateStudies/docsandreports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\homer\ClimateStudies\docsandreports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FE80FA1-2CFF-4394-A6F2-1147BE870DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03822EE1-1546-4521-B214-988F2AFC1AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8235" yWindow="1935" windowWidth="27585" windowHeight="16320" xr2:uid="{7E555591-D244-41B1-826E-35EFBAB279F7}"/>
+    <workbookView xWindow="10500" yWindow="210" windowWidth="27585" windowHeight="16320" xr2:uid="{7E555591-D244-41B1-826E-35EFBAB279F7}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationMasterList" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="84">
   <si>
     <t>KCC</t>
   </si>
@@ -269,6 +269,27 @@
   </si>
   <si>
     <t>Coeur d'Alene/Kootenai, ID</t>
+  </si>
+  <si>
+    <t>Wadena, MN</t>
+  </si>
+  <si>
+    <t>Bismarck, ND</t>
+  </si>
+  <si>
+    <t>Marlinton, WV</t>
+  </si>
+  <si>
+    <t>Richmond, VA</t>
+  </si>
+  <si>
+    <t>Raleigh, NC</t>
+  </si>
+  <si>
+    <t>Atlanta, GA</t>
+  </si>
+  <si>
+    <t>Lancaster, PA</t>
   </si>
 </sst>
 </file>
@@ -754,11 +775,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0019611-06D4-42E5-A194-8B884DB54B83}">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B57" sqref="B57"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,11 +1742,431 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="1"/>
+      <c r="A57" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" s="3">
+        <v>46.441670000000002</v>
+      </c>
+      <c r="D57" s="4">
+        <v>95.136669999999995</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" s="3">
+        <v>46.808329999999998</v>
+      </c>
+      <c r="D58" s="4">
+        <v>100.7833</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59" s="3">
+        <v>38.223329999999997</v>
+      </c>
+      <c r="D59" s="4">
+        <v>80.094999999999999</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="3">
+        <v>37.54</v>
+      </c>
+      <c r="D60" s="4">
+        <v>77.436670000000007</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61" s="3">
+        <v>35.78</v>
+      </c>
+      <c r="D61" s="4">
+        <v>78.638329999999996</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62" s="3">
+        <v>33.748330000000003</v>
+      </c>
+      <c r="D62" s="4">
+        <v>84.388329999999996</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63" s="3">
+        <v>40.038330000000002</v>
+      </c>
+      <c r="D63" s="4">
+        <v>76.305000000000007</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="1"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="1"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="1"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="1"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="1"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="1"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="2"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="1"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="1"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="1"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="2"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="1"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="2"/>
+      <c r="B81" s="8"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="1"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="2"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="1"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="2"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="1"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="2"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="2"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="2"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="1"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
+      <c r="B87" s="8"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="1"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="2"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="1"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="2"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="1"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="2"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="1"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="2"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="2"/>
+      <c r="B92" s="8"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="1"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="2"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="1"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="2"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="1"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="2"/>
+      <c r="B95" s="8"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="1"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="2"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="1"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="2"/>
+      <c r="B97" s="8"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="1"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="2"/>
+      <c r="B98" s="8"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="1"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="2"/>
+      <c r="B99" s="8"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="1"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="1"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="2"/>
+      <c r="B101" s="8"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="1"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+      <c r="B102" s="8"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="1"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="2"/>
+      <c r="B103" s="8"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="1"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+      <c r="B104" s="8"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="1"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+      <c r="B105" s="8"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="1"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+      <c r="B106" s="8"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="1"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+      <c r="B107" s="8"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:A57" xr:uid="{A0019611-06D4-42E5-A194-8B884DB54B83}"/>

</xml_diff>

<commit_message>
Committing all locational variance runs
</commit_message>
<xml_diff>
--- a/ClimateStudies/docsandreports/uRXClimateStudiesMasterFile.xlsx
+++ b/ClimateStudies/docsandreports/uRXClimateStudiesMasterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\homer\ClimateStudies\docsandreports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03822EE1-1546-4521-B214-988F2AFC1AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9470ADE-A4CB-4E09-A869-7908E567F1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10500" yWindow="210" windowWidth="27585" windowHeight="16320" xr2:uid="{7E555591-D244-41B1-826E-35EFBAB279F7}"/>
+    <workbookView xWindow="18660" yWindow="375" windowWidth="14805" windowHeight="15915" xr2:uid="{7E555591-D244-41B1-826E-35EFBAB279F7}"/>
   </bookViews>
   <sheets>
     <sheet name="LocationMasterList" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -459,6 +459,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -778,8 +784,8 @@
   <dimension ref="A1:H107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,13 +817,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="C2" s="6">
-        <v>64.643330000000006</v>
+        <v>61.218330000000002</v>
       </c>
       <c r="D2" s="7">
-        <v>147.0633</v>
+        <v>149.9</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>33</v>
@@ -842,16 +848,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="C4" s="3">
-        <v>44.6</v>
+        <v>33.748330000000003</v>
       </c>
       <c r="D4" s="4">
-        <v>123.21</v>
+        <v>84.388329999999996</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>33</v>
@@ -859,16 +865,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="C5" s="3">
-        <v>48.606670000000001</v>
+        <v>44.801670000000001</v>
       </c>
       <c r="D5" s="4">
-        <v>108.94670000000001</v>
+        <v>68.77167</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>33</v>
@@ -876,16 +882,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C6" s="3">
-        <v>29.95167</v>
+        <v>44.06</v>
       </c>
       <c r="D6" s="4">
-        <v>90.071669999999997</v>
+        <v>121.2467</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>33</v>
@@ -893,16 +899,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3">
-        <v>32.104999999999997</v>
+        <v>44.6</v>
       </c>
       <c r="D7" s="4">
-        <v>102.18170000000001</v>
+        <v>123.21</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>33</v>
@@ -913,13 +919,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C8" s="3">
-        <v>35.931669999999997</v>
+        <v>33.518329999999999</v>
       </c>
       <c r="D8" s="4">
-        <v>84.31</v>
+        <v>86.81</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>33</v>
@@ -930,13 +936,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="C9" s="3">
-        <v>43.49333</v>
+        <v>46.808329999999998</v>
       </c>
       <c r="D9" s="4">
-        <v>112.04</v>
+        <v>100.7833</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>33</v>
@@ -947,13 +953,13 @@
         <v>27</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3">
-        <v>43.615000000000002</v>
+        <v>48.606670000000001</v>
       </c>
       <c r="D10" s="4">
-        <v>116.2017</v>
+        <v>108.94670000000001</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>33</v>
@@ -961,16 +967,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="3">
-        <v>41.878329999999998</v>
+        <v>43.615000000000002</v>
       </c>
       <c r="D11" s="4">
-        <v>87.63</v>
+        <v>116.2017</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>33</v>
@@ -978,16 +984,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="C12" s="3">
-        <v>32.693330000000003</v>
+        <v>41.76</v>
       </c>
       <c r="D12" s="4">
-        <v>114.6283</v>
+        <v>70.083330000000004</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>33</v>
@@ -995,16 +1001,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C13" s="3">
-        <v>35.198329999999999</v>
+        <v>44.476669999999999</v>
       </c>
       <c r="D13" s="4">
-        <v>111.64830000000001</v>
+        <v>73.203329999999994</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>33</v>
@@ -1012,16 +1018,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="C14" s="3">
-        <v>25.286670000000001</v>
+        <v>35.4</v>
       </c>
       <c r="D14" s="4">
-        <v>80.898330000000001</v>
+        <v>119.47</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>33</v>
@@ -1029,16 +1035,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="C15" s="3">
-        <v>25.761669999999999</v>
+        <v>39.163330000000002</v>
       </c>
       <c r="D15" s="4">
-        <v>80.191670000000002</v>
+        <v>119.7667</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>33</v>
@@ -1046,16 +1052,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>65</v>
       </c>
       <c r="C16" s="3">
-        <v>38.581670000000003</v>
+        <v>41.14</v>
       </c>
       <c r="D16" s="4">
-        <v>121.495</v>
+        <v>104.82</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>33</v>
@@ -1063,16 +1069,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3">
-        <v>35.4</v>
+        <v>41.878329999999998</v>
       </c>
       <c r="D17" s="4">
-        <v>119.47</v>
+        <v>87.63</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>33</v>
@@ -1080,16 +1086,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C18" s="3">
-        <v>48.36833</v>
+        <v>40.918329999999997</v>
       </c>
       <c r="D18" s="4">
-        <v>124.625</v>
+        <v>111.4</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>33</v>
@@ -1097,16 +1103,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="C19" s="3">
-        <v>46.138330000000003</v>
+        <v>47.86833</v>
       </c>
       <c r="D19" s="4">
-        <v>122.9383</v>
+        <v>116.4667</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>33</v>
@@ -1131,16 +1137,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C21" s="3">
-        <v>43.04833</v>
+        <v>39.961669999999998</v>
       </c>
       <c r="D21" s="4">
-        <v>76.14667</v>
+        <v>82.998329999999996</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>33</v>
@@ -1148,16 +1154,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C22" s="3">
-        <v>19.723330000000001</v>
+        <v>38.869999999999997</v>
       </c>
       <c r="D22" s="4">
-        <v>155.08670000000001</v>
+        <v>106.9883</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>33</v>
@@ -1165,16 +1171,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C23" s="3">
-        <v>22.081669999999999</v>
+        <v>41.586669999999998</v>
       </c>
       <c r="D23" s="4">
-        <v>159.52500000000001</v>
+        <v>93.625</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>33</v>
@@ -1182,16 +1188,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C24" s="3">
-        <v>32.29833</v>
+        <v>42.331670000000003</v>
       </c>
       <c r="D24" s="4">
-        <v>90.185000000000002</v>
+        <v>83.045000000000002</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>33</v>
@@ -1199,16 +1205,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="C25" s="3">
-        <v>35.15</v>
+        <v>64.643330000000006</v>
       </c>
       <c r="D25" s="4">
-        <v>90.048330000000007</v>
+        <v>147.0633</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>33</v>
@@ -1216,16 +1222,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C26" s="3">
-        <v>46.534999999999997</v>
+        <v>25.286670000000001</v>
       </c>
       <c r="D26" s="4">
-        <v>87.405000000000001</v>
+        <v>80.898330000000001</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>33</v>
@@ -1233,16 +1239,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C27" s="3">
-        <v>38.255000000000003</v>
+        <v>35.198329999999999</v>
       </c>
       <c r="D27" s="4">
-        <v>104.6083</v>
+        <v>111.64830000000001</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>33</v>
@@ -1250,16 +1256,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C28" s="3">
-        <v>38.869999999999997</v>
+        <v>47.505000000000003</v>
       </c>
       <c r="D28" s="4">
-        <v>106.9883</v>
+        <v>111.3</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>33</v>
@@ -1267,16 +1273,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C29" s="3">
-        <v>35.880000000000003</v>
+        <v>19.723330000000001</v>
       </c>
       <c r="D29" s="4">
-        <v>106.30329999999999</v>
+        <v>155.08670000000001</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>33</v>
@@ -1284,16 +1290,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C30" s="3">
-        <v>61.218330000000002</v>
+        <v>43.49333</v>
       </c>
       <c r="D30" s="4">
-        <v>149.9</v>
+        <v>112.04</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>33</v>
@@ -1301,16 +1307,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C31" s="3">
-        <v>44.06</v>
+        <v>32.29833</v>
       </c>
       <c r="D31" s="4">
-        <v>121.2467</v>
+        <v>90.185000000000002</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>33</v>
@@ -1318,16 +1324,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C32" s="3">
-        <v>40.918329999999997</v>
+        <v>22.081669999999999</v>
       </c>
       <c r="D32" s="4">
-        <v>111.4</v>
+        <v>159.52500000000001</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>33</v>
@@ -1335,16 +1341,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="C33" s="3">
-        <v>35.468330000000002</v>
+        <v>40.038330000000002</v>
       </c>
       <c r="D33" s="4">
-        <v>97.516670000000005</v>
+        <v>76.305000000000007</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>33</v>
@@ -1352,16 +1358,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C34" s="3">
-        <v>34.746670000000002</v>
+        <v>27.503329999999998</v>
       </c>
       <c r="D34" s="4">
-        <v>92.29</v>
+        <v>99.508330000000001</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>33</v>
@@ -1369,16 +1375,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C35" s="3">
-        <v>33.518329999999999</v>
+        <v>36.17</v>
       </c>
       <c r="D35" s="4">
-        <v>86.81</v>
+        <v>115.14</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>33</v>
@@ -1386,16 +1392,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C36" s="3">
-        <v>30.695</v>
+        <v>40.813330000000001</v>
       </c>
       <c r="D36" s="4">
-        <v>88.04</v>
+        <v>96.703329999999994</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>33</v>
@@ -1403,16 +1409,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C37" s="3">
-        <v>44.801670000000001</v>
+        <v>34.746670000000002</v>
       </c>
       <c r="D37" s="4">
-        <v>68.77167</v>
+        <v>92.29</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>33</v>
@@ -1420,16 +1426,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="C38" s="3">
-        <v>44.476669999999999</v>
+        <v>46.138330000000003</v>
       </c>
       <c r="D38" s="4">
-        <v>73.203329999999994</v>
+        <v>122.9383</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>33</v>
@@ -1437,16 +1443,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C39" s="3">
-        <v>41.676670000000001</v>
+        <v>35.880000000000003</v>
       </c>
       <c r="D39" s="4">
-        <v>86.251670000000004</v>
+        <v>106.30329999999999</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>33</v>
@@ -1454,16 +1460,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="C40" s="3">
-        <v>39.961669999999998</v>
+        <v>38.223329999999997</v>
       </c>
       <c r="D40" s="4">
-        <v>82.998329999999996</v>
+        <v>80.094999999999999</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>33</v>
@@ -1471,16 +1477,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C41" s="3">
-        <v>42.331670000000003</v>
+        <v>46.534999999999997</v>
       </c>
       <c r="D41" s="4">
-        <v>83.045000000000002</v>
+        <v>87.405000000000001</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>33</v>
@@ -1488,16 +1494,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C42" s="3">
-        <v>41.586669999999998</v>
+        <v>42.32667</v>
       </c>
       <c r="D42" s="4">
-        <v>93.625</v>
+        <v>122.875</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>33</v>
@@ -1505,16 +1511,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="C43" s="3">
-        <v>40.813330000000001</v>
+        <v>35.15</v>
       </c>
       <c r="D43" s="4">
-        <v>96.703329999999994</v>
+        <v>90.048330000000007</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>33</v>
@@ -1522,16 +1528,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C44" s="3">
-        <v>47.505000000000003</v>
+        <v>25.761669999999999</v>
       </c>
       <c r="D44" s="4">
-        <v>111.3</v>
+        <v>80.191670000000002</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>33</v>
@@ -1539,16 +1545,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="C45" s="3">
-        <v>41.14</v>
+        <v>32.104999999999997</v>
       </c>
       <c r="D45" s="4">
-        <v>104.82</v>
+        <v>102.18170000000001</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>33</v>
@@ -1556,16 +1562,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C46" s="3">
-        <v>44.08</v>
+        <v>30.695</v>
       </c>
       <c r="D46" s="4">
-        <v>103.2317</v>
+        <v>88.04</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>33</v>
@@ -1573,16 +1579,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C47" s="3">
-        <v>36.17</v>
+        <v>46.731670000000001</v>
       </c>
       <c r="D47" s="4">
-        <v>115.14</v>
+        <v>117</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>33</v>
@@ -1590,16 +1596,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="C48" s="3">
-        <v>33.448329999999999</v>
+        <v>48.36833</v>
       </c>
       <c r="D48" s="4">
-        <v>112.0733</v>
+        <v>124.625</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>33</v>
@@ -1607,16 +1613,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="C49" s="3">
-        <v>39.163330000000002</v>
+        <v>29.95167</v>
       </c>
       <c r="D49" s="4">
-        <v>119.7667</v>
+        <v>90.071669999999997</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>33</v>
@@ -1624,16 +1630,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="C50" s="3">
-        <v>42.32667</v>
+        <v>35.931669999999997</v>
       </c>
       <c r="D50" s="4">
-        <v>122.875</v>
+        <v>84.31</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>33</v>
@@ -1641,16 +1647,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C51" s="3">
-        <v>40.586669999999998</v>
+        <v>35.468330000000002</v>
       </c>
       <c r="D51" s="4">
-        <v>122.3917</v>
+        <v>97.516670000000005</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>33</v>
@@ -1658,16 +1664,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C52" s="3">
-        <v>34.528329999999997</v>
+        <v>33.448329999999999</v>
       </c>
       <c r="D52" s="4">
-        <v>112.45</v>
+        <v>112.0733</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>33</v>
@@ -1675,16 +1681,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C53" s="3">
-        <v>27.503329999999998</v>
+        <v>34.528329999999997</v>
       </c>
       <c r="D53" s="4">
-        <v>99.508330000000001</v>
+        <v>112.45</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>33</v>
@@ -1692,16 +1698,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="C54" s="3">
-        <v>41.76</v>
+        <v>38.255000000000003</v>
       </c>
       <c r="D54" s="4">
-        <v>70.083330000000004</v>
+        <v>104.6083</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>33</v>
@@ -1709,16 +1715,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C55" s="3">
-        <v>46.731670000000001</v>
+        <v>35.78</v>
       </c>
       <c r="D55" s="4">
-        <v>117</v>
+        <v>78.638329999999996</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>33</v>
@@ -1726,16 +1732,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C56" s="3">
-        <v>47.86833</v>
+        <v>44.08</v>
       </c>
       <c r="D56" s="4">
-        <v>116.4667</v>
+        <v>103.2317</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>33</v>
@@ -1743,16 +1749,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C57" s="3">
-        <v>46.441670000000002</v>
+        <v>40.586669999999998</v>
       </c>
       <c r="D57" s="4">
-        <v>95.136669999999995</v>
+        <v>122.3917</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>33</v>
@@ -1760,16 +1766,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C58" s="3">
-        <v>46.808329999999998</v>
+        <v>37.54</v>
       </c>
       <c r="D58" s="4">
-        <v>100.7833</v>
+        <v>77.436670000000007</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>33</v>
@@ -1777,16 +1783,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>79</v>
+        <v>28</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="C59" s="3">
-        <v>38.223329999999997</v>
+        <v>38.581670000000003</v>
       </c>
       <c r="D59" s="4">
-        <v>80.094999999999999</v>
+        <v>121.495</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>33</v>
@@ -1794,16 +1800,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="C60" s="3">
-        <v>37.54</v>
+        <v>41.676670000000001</v>
       </c>
       <c r="D60" s="4">
-        <v>77.436670000000007</v>
+        <v>86.251670000000004</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>33</v>
@@ -1811,16 +1817,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="C61" s="3">
-        <v>35.78</v>
+        <v>43.04833</v>
       </c>
       <c r="D61" s="4">
-        <v>78.638329999999996</v>
+        <v>76.14667</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>33</v>
@@ -1828,16 +1834,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C62" s="3">
-        <v>33.748330000000003</v>
+        <v>46.441670000000002</v>
       </c>
       <c r="D62" s="4">
-        <v>84.388329999999996</v>
+        <v>95.136669999999995</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>33</v>
@@ -1845,16 +1851,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="C63" s="3">
-        <v>40.038330000000002</v>
+        <v>32.693330000000003</v>
       </c>
       <c r="D63" s="4">
-        <v>76.305000000000007</v>
+        <v>114.6283</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>33</v>
@@ -2170,6 +2176,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:A57" xr:uid="{A0019611-06D4-42E5-A194-8B884DB54B83}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F63">
+    <sortCondition ref="B1:B63"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>